<commit_message>
added resultstable in csv and edited dataset slighlty
</commit_message>
<xml_diff>
--- a/Full Dataset.xlsx
+++ b/Full Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzlol\Documents\GitHub\final_year_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBDCC52-589F-49EF-BE4D-0775E87BA8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920009E-9D5F-449A-8D5D-85BDBDE2028D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8104B03C-3216-4DCF-A532-412FD289F5DD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8104B03C-3216-4DCF-A532-412FD289F5DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="318">
   <si>
     <t>Class Weights</t>
   </si>
@@ -986,13 +986,16 @@
   </si>
   <si>
     <t>192|5240|69|174</t>
+  </si>
+  <si>
+    <t>0|0|0|0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,8 +1023,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1036,6 +1046,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1088,12 +1103,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -1103,10 +1119,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1421,32 +1439,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DABE3BF-0B38-41CB-992B-78482D035AE6}">
   <dimension ref="B1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="89" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="18.5546875" customWidth="1"/>
-    <col min="17" max="17" width="60.88671875" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="60.85546875" customWidth="1"/>
     <col min="19" max="19" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>79</v>
       </c>
@@ -1463,7 +1481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1507,11 +1525,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1546,11 +1572,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1582,11 +1616,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
       <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1618,11 +1660,19 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1654,11 +1704,19 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
       <c r="F7" s="5" t="s">
         <v>2</v>
       </c>
@@ -1690,11 +1748,19 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
       <c r="F8" s="5" t="s">
         <v>2</v>
       </c>
@@ -1726,11 +1792,19 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
       <c r="F9" s="5" t="s">
         <v>2</v>
       </c>
@@ -1762,11 +1836,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
       <c r="F10" s="5" t="s">
         <v>2</v>
       </c>
@@ -1798,11 +1880,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
       <c r="F11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1834,11 +1924,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
       <c r="F12" s="5" t="s">
         <v>2</v>
       </c>
@@ -1870,11 +1968,19 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
       <c r="F13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1906,11 +2012,19 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
       <c r="F14" s="5" t="s">
         <v>2</v>
       </c>
@@ -1942,11 +2056,19 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
       <c r="F15" s="5" t="s">
         <v>2</v>
       </c>
@@ -1978,11 +2100,19 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
       <c r="F16" s="5" t="s">
         <v>2</v>
       </c>
@@ -2014,11 +2144,19 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
       <c r="F17" s="5" t="s">
         <v>2</v>
       </c>
@@ -2050,11 +2188,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
       <c r="F18" s="5" t="s">
         <v>2</v>
       </c>
@@ -2086,11 +2232,19 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
       <c r="F19" s="5" t="s">
         <v>3</v>
       </c>
@@ -2100,21 +2254,41 @@
       <c r="H19" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="I19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O19">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="2"/>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
       <c r="F20" s="5" t="s">
         <v>3</v>
       </c>
@@ -2124,21 +2298,41 @@
       <c r="H20" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="I20" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O20">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
       <c r="F21" s="5" t="s">
         <v>3</v>
       </c>
@@ -2148,21 +2342,41 @@
       <c r="H21" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
+      <c r="I21" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O21">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
       <c r="F22" s="5" t="s">
         <v>3</v>
       </c>
@@ -2172,21 +2386,41 @@
       <c r="H22" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
+      <c r="I22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O22">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
       <c r="F23" s="5" t="s">
         <v>3</v>
       </c>
@@ -2196,21 +2430,41 @@
       <c r="H23" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
+      <c r="I23" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O23">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
       <c r="F24" s="5" t="s">
         <v>3</v>
       </c>
@@ -2220,21 +2474,41 @@
       <c r="H24" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
+      <c r="I24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O24">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
       <c r="F25" s="5" t="s">
         <v>3</v>
       </c>
@@ -2244,21 +2518,41 @@
       <c r="H25" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+      <c r="I25" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O25">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
       <c r="F26" s="5" t="s">
         <v>3</v>
       </c>
@@ -2268,21 +2562,41 @@
       <c r="H26" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+      <c r="I26" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O26">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
       <c r="F27" s="5" t="s">
         <v>3</v>
       </c>
@@ -2292,21 +2606,41 @@
       <c r="H27" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
+      <c r="I27" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O27">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
       <c r="F28" s="5" t="s">
         <v>3</v>
       </c>
@@ -2316,21 +2650,41 @@
       <c r="H28" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
+      <c r="I28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O28">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
       <c r="F29" s="5" t="s">
         <v>3</v>
       </c>
@@ -2340,21 +2694,41 @@
       <c r="H29" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
+      <c r="I29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O29">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2</v>
+      </c>
       <c r="F30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2364,21 +2738,41 @@
       <c r="H30" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
+      <c r="I30" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O30">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
       <c r="F31" s="5" t="s">
         <v>3</v>
       </c>
@@ -2388,21 +2782,41 @@
       <c r="H31" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
+      <c r="I31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O31">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="2"/>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
       <c r="F32" s="5" t="s">
         <v>3</v>
       </c>
@@ -2412,21 +2826,41 @@
       <c r="H32" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
+      <c r="I32" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O32">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
       <c r="F33" s="5" t="s">
         <v>3</v>
       </c>
@@ -2436,21 +2870,41 @@
       <c r="H33" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
+      <c r="I33" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N33" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O33">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2</v>
+      </c>
       <c r="F34" s="5" t="s">
         <v>3</v>
       </c>
@@ -2460,21 +2914,41 @@
       <c r="H34" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
+      <c r="I34" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O34">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
       <c r="F35" s="5" t="s">
         <v>4</v>
       </c>
@@ -2484,21 +2958,41 @@
       <c r="H35" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
+      <c r="I35" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N35" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O35">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
       <c r="F36" s="5" t="s">
         <v>4</v>
       </c>
@@ -2508,21 +3002,41 @@
       <c r="H36" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
+      <c r="I36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O36">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
       <c r="F37" s="5" t="s">
         <v>4</v>
       </c>
@@ -2532,21 +3046,41 @@
       <c r="H37" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
+      <c r="I37" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O37">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
       <c r="F38" s="5" t="s">
         <v>4</v>
       </c>
@@ -2556,21 +3090,41 @@
       <c r="H38" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="I38" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O38">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
       <c r="F39" s="5" t="s">
         <v>4</v>
       </c>
@@ -2580,21 +3134,41 @@
       <c r="H39" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
+      <c r="I39" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M39" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O39">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="2"/>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
       <c r="F40" s="5" t="s">
         <v>4</v>
       </c>
@@ -2604,21 +3178,41 @@
       <c r="H40" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
+      <c r="I40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N40" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O40">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
       <c r="F41" s="5" t="s">
         <v>4</v>
       </c>
@@ -2628,21 +3222,41 @@
       <c r="H41" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
+      <c r="I41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N41" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O41">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
       <c r="F42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2652,21 +3266,41 @@
       <c r="H42" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
+      <c r="I42" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N42" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O42">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
       <c r="F43" s="5" t="s">
         <v>4</v>
       </c>
@@ -2676,21 +3310,41 @@
       <c r="H43" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
+      <c r="I43" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M43" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N43" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O43">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="2"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2</v>
+      </c>
       <c r="F44" s="5" t="s">
         <v>4</v>
       </c>
@@ -2700,21 +3354,41 @@
       <c r="H44" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
+      <c r="I44" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M44" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N44" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O44">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B45" s="2"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="3"/>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
       <c r="F45" s="5" t="s">
         <v>4</v>
       </c>
@@ -2724,21 +3398,41 @@
       <c r="H45" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
+      <c r="I45" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M45" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N45" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O45">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2</v>
+      </c>
       <c r="F46" s="5" t="s">
         <v>4</v>
       </c>
@@ -2748,21 +3442,41 @@
       <c r="H46" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
+      <c r="I46" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M46" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N46" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O46">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
       <c r="F47" s="5" t="s">
         <v>4</v>
       </c>
@@ -2772,21 +3486,41 @@
       <c r="H47" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
+      <c r="I47" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M47" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N47" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O47">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="2"/>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2</v>
+      </c>
       <c r="F48" s="5" t="s">
         <v>4</v>
       </c>
@@ -2796,21 +3530,41 @@
       <c r="H48" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
+      <c r="I48" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M48" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N48" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O48">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="3"/>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
       <c r="F49" s="5" t="s">
         <v>4</v>
       </c>
@@ -2820,21 +3574,41 @@
       <c r="H49" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
+      <c r="I49" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L49" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M49" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N49" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O49">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2</v>
+      </c>
       <c r="F50" s="5" t="s">
         <v>4</v>
       </c>
@@ -2844,21 +3618,41 @@
       <c r="H50" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
+      <c r="I50" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K50" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L50" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="N50" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="O50">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
       <c r="F51" s="5" t="s">
         <v>5</v>
       </c>
@@ -2890,11 +3684,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="2"/>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2</v>
+      </c>
       <c r="F52" s="5" t="s">
         <v>5</v>
       </c>
@@ -2926,11 +3728,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="3"/>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
       <c r="F53" s="5" t="s">
         <v>5</v>
       </c>
@@ -2962,11 +3772,19 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2</v>
+      </c>
       <c r="F54" s="5" t="s">
         <v>5</v>
       </c>
@@ -2998,11 +3816,19 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B55" s="3"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
       <c r="F55" s="5" t="s">
         <v>5</v>
       </c>
@@ -3034,11 +3860,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B56" s="3"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="2"/>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2</v>
+      </c>
       <c r="F56" s="5" t="s">
         <v>5</v>
       </c>
@@ -3070,11 +3904,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B57" s="3"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="3"/>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
       <c r="F57" s="5" t="s">
         <v>5</v>
       </c>
@@ -3106,11 +3948,19 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B58" s="3"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2</v>
+      </c>
       <c r="F58" s="5" t="s">
         <v>5</v>
       </c>
@@ -3142,11 +3992,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B59" s="2"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
@@ -3178,11 +4036,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B60" s="2"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="2"/>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
+        <v>2</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <v>1</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2</v>
+      </c>
       <c r="F60" s="5" t="s">
         <v>5</v>
       </c>
@@ -3214,11 +4080,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B61" s="2"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="3"/>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="2">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
       <c r="F61" s="5" t="s">
         <v>5</v>
       </c>
@@ -3250,11 +4124,19 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B62" s="2"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+      <c r="E62" s="2">
+        <v>2</v>
+      </c>
       <c r="F62" s="5" t="s">
         <v>5</v>
       </c>
@@ -3286,11 +4168,19 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>2</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2</v>
+      </c>
+      <c r="D63" s="3">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
       <c r="F63" s="5" t="s">
         <v>5</v>
       </c>
@@ -3322,11 +4212,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="2"/>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>2</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2</v>
+      </c>
+      <c r="D64" s="3">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2</v>
+      </c>
       <c r="F64" s="5" t="s">
         <v>5</v>
       </c>
@@ -3358,11 +4256,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="3"/>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="2">
+        <v>2</v>
+      </c>
+      <c r="C65" s="2">
+        <v>2</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
+      <c r="E65" s="3">
+        <v>1</v>
+      </c>
       <c r="F65" s="5" t="s">
         <v>5</v>
       </c>
@@ -3394,11 +4300,19 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
+        <v>2</v>
+      </c>
+      <c r="C66" s="4">
+        <v>2</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4">
+        <v>2</v>
+      </c>
       <c r="F66" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>